<commit_message>
fix : RR001 parts PartNo fix
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/RR001.xlsx
+++ b/機械設計/_BOM/RR001.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52C5129C-EAA0-448C-B90A-48EB072F038F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3E15ACE4-AD88-4F7C-A774-73DCA1F6466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17970" yWindow="13980" windowWidth="14400" windowHeight="10845" xr2:uid="{7EC68FF2-9777-4108-9020-7FCCEE109C72}"/>
+    <workbookView xWindow="-28920" yWindow="-2790" windowWidth="29040" windowHeight="15840" xr2:uid="{7EC68FF2-9777-4108-9020-7FCCEE109C72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="932" windowWidth="960" windowHeight="723" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-186" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -374,8 +374,13 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F2BAFE31-B20A-47E5-8260-29B914D5E271}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5EEC1257-520C-4BC4-AB31-84AA4BB3E573}" diskRevisions="1" version="2">
   <header guid="{F2BAFE31-B20A-47E5-8260-29B914D5E271}" dateTime="2023-07-12T19:08:52" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5EEC1257-520C-4BC4-AB31-84AA4BB3E573}" dateTime="2023-07-13T14:12:27" maxSheetId="2" userName="DESKTOP-1" r:id="rId2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -385,6 +390,13 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" action="delete"/>
+  <rcv guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,7 +702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A53796-ED47-4E09-BA12-0EC1DDE61B00}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1613,7 +1627,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}">
+    <customSheetView guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" scale="130">
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>

<commit_message>
add : RL001 subasm and parts profile fix
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/RR001.xlsx
+++ b/機械設計/_BOM/RR001.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{3E15ACE4-AD88-4F7C-A774-73DCA1F6466D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{636027E4-07A7-4C0E-A06B-D61089860912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2790" windowWidth="29040" windowHeight="15840" xr2:uid="{7EC68FF2-9777-4108-9020-7FCCEE109C72}"/>
+    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{C1D8E0BB-A9BF-4545-B8E8-F52391355FF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-186" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{C077F416-FB9C-4645-9EBB-E4D407545260}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="85">
   <si>
     <t>種類</t>
   </si>
@@ -122,6 +122,15 @@
     <t>R-P001</t>
   </si>
   <si>
+    <t>足側板内側</t>
+  </si>
+  <si>
+    <t>A2017</t>
+  </si>
+  <si>
+    <t>R-P002</t>
+  </si>
+  <si>
     <t>足機構固定板</t>
   </si>
   <si>
@@ -134,42 +143,36 @@
     <t>黒</t>
   </si>
   <si>
+    <t>R-P003</t>
+  </si>
+  <si>
+    <t>足機構上面カバー</t>
+  </si>
+  <si>
+    <t>R-P004</t>
+  </si>
+  <si>
+    <t>足機構主柱</t>
+  </si>
+  <si>
     <t>RR</t>
   </si>
   <si>
     <t>RR-P001</t>
   </si>
   <si>
-    <t>足側板</t>
-  </si>
-  <si>
-    <t>A2017</t>
+    <t>足側板右外側</t>
   </si>
   <si>
     <t>RR-P002</t>
   </si>
   <si>
-    <t>RR-P003</t>
-  </si>
-  <si>
-    <t>足機構上面カバー</t>
-  </si>
-  <si>
-    <t>RR-P004</t>
-  </si>
-  <si>
     <t>右足機構側面充填樹脂</t>
   </si>
   <si>
     <t>ｴﾎﾟｷｼ樹脂(充填剤なし)</t>
   </si>
   <si>
-    <t>RR-P005</t>
-  </si>
-  <si>
-    <t>足機構主柱</t>
-  </si>
-  <si>
     <t>購入品</t>
   </si>
   <si>
@@ -197,6 +200,36 @@
     <t>タイミングベルト</t>
   </si>
   <si>
+    <t>CB2.6-5</t>
+  </si>
+  <si>
+    <t>SCM435</t>
+  </si>
+  <si>
+    <t>六角穴付ﾎﾞﾙﾄ</t>
+  </si>
+  <si>
+    <t>1日目</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>マブチ</t>
+  </si>
+  <si>
+    <t>RS380-PH</t>
+  </si>
+  <si>
+    <t>材料 &lt;指定なし&gt;</t>
+  </si>
+  <si>
+    <t>馬渕モータ RS380PH</t>
+  </si>
+  <si>
+    <t>電動機</t>
+  </si>
+  <si>
     <t>KHK</t>
   </si>
   <si>
@@ -227,15 +260,9 @@
     <t>CBSTBR3-6</t>
   </si>
   <si>
-    <t>SCM435</t>
-  </si>
-  <si>
     <t>超極低頭ﾎﾞﾙﾄ</t>
   </si>
   <si>
-    <t>1日目</t>
-  </si>
-  <si>
     <t>MPFZ10-8</t>
   </si>
   <si>
@@ -243,30 +270,6 @@
   </si>
   <si>
     <t>無給油ﾌﾞｯｼｭ</t>
-  </si>
-  <si>
-    <t>CB2.6-5</t>
-  </si>
-  <si>
-    <t>六角穴付ﾎﾞﾙﾄ</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>マブチ</t>
-  </si>
-  <si>
-    <t>RS380-PH</t>
-  </si>
-  <si>
-    <t>材料 &lt;指定なし&gt;</t>
-  </si>
-  <si>
-    <t>馬渕モータ RS380PH</t>
-  </si>
-  <si>
-    <t>電動機</t>
   </si>
   <si>
     <t>組立品</t>
@@ -374,13 +377,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5EEC1257-520C-4BC4-AB31-84AA4BB3E573}" diskRevisions="1" version="2">
-  <header guid="{F2BAFE31-B20A-47E5-8260-29B914D5E271}" dateTime="2023-07-12T19:08:52" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{5EEC1257-520C-4BC4-AB31-84AA4BB3E573}" dateTime="2023-07-13T14:12:27" maxSheetId="2" userName="DESKTOP-1" r:id="rId2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2F1484D2-B53A-4C28-B303-D0C700A68DAB}">
+  <header guid="{2F1484D2-B53A-4C28-B303-D0C700A68DAB}" dateTime="2023-07-13T14:18:11" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -392,15 +390,10 @@
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
 </file>
 
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" action="delete"/>
-  <rcv guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" action="add"/>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+  <userInfo guid="{2F1484D2-B53A-4C28-B303-D0C700A68DAB}" name="DESKTOP-1" id="-1212795428" dateTime="2023-07-13T14:18:43"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -699,12 +692,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4A53796-ED47-4E09-BA12-0EC1DDE61B00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16247DFC-FCB6-4707-A758-3C064142A299}">
   <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -849,26 +840,26 @@
         <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="3"/>
       <c r="N3" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>23</v>
@@ -885,37 +876,37 @@
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="3"/>
       <c r="N4" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>23</v>
@@ -932,18 +923,18 @@
         <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -979,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>36</v>
@@ -990,13 +981,13 @@
         <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="H6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1026,18 +1017,18 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1">
         <v>1</v>
@@ -1073,7 +1064,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>41</v>
@@ -1084,13 +1075,13 @@
         <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1117,21 +1108,21 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" s="1">
         <v>7</v>
@@ -1139,18 +1130,18 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9" s="3"/>
       <c r="N9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>23</v>
@@ -1164,21 +1155,21 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -1188,7 +1179,7 @@
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="3"/>
@@ -1213,15 +1204,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>53</v>
@@ -1230,66 +1219,60 @@
         <v>54</v>
       </c>
       <c r="H11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="M11" s="3">
-        <v>150</v>
+        <v>642</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="H12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="K12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M12" s="3">
-        <v>300</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="3"/>
       <c r="N12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1303,74 +1286,82 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="E13" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="L13" s="1"/>
       <c r="M13" s="3">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="O13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="Q13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="R13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H14" s="1">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="M14" s="3">
-        <v>280</v>
+        <v>300</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>23</v>
@@ -1385,33 +1376,33 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H15" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="M15" s="3">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>23</v>
@@ -1426,33 +1417,33 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="M16" s="3">
-        <v>642</v>
+        <v>280</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>23</v>
@@ -1467,34 +1458,34 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H17" s="1">
         <v>2</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>74</v>
-      </c>
+      <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" s="3">
+        <v>500</v>
+      </c>
       <c r="N17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1508,21 +1499,21 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
@@ -1531,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1549,21 +1540,21 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
@@ -1588,21 +1579,21 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="H20" s="1">
         <v>1</v>
@@ -1627,8 +1618,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3752E983-C2A4-443E-9EE5-C297EE2BA75F}" scale="130">
-      <selection activeCell="B6" sqref="B6"/>
+    <customSheetView guid="{C077F416-FB9C-4645-9EBB-E4D407545260}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>